<commit_message>
A nice and well needed gitignore.
</commit_message>
<xml_diff>
--- a/gantt-chart-masters-thesis.xlsx
+++ b/gantt-chart-masters-thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\edu\Masters-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D59456C-ECD8-4729-83CF-53539B9322C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48E9CE6-8BC3-4CCE-81C8-DA71B667944A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{B2266D63-D624-47C8-9EC7-BE94EEB4DD94}"/>
   </bookViews>
@@ -199,7 +199,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,13 +220,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +285,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -298,6 +304,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -310,49 +346,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -761,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E332D38E-AECF-4C52-8405-774533E18050}">
-  <dimension ref="A5:AK34"/>
+  <dimension ref="A5:AK35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -779,22 +794,22 @@
   <sheetData>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:37" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:37" ht="18" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -806,51 +821,51 @@
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
-      <c r="AI10" s="9"/>
-      <c r="AJ10" s="9"/>
-      <c r="AK10" s="9"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="19"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
+      <c r="AF10" s="19"/>
+      <c r="AG10" s="19"/>
+      <c r="AH10" s="19"/>
+      <c r="AI10" s="19"/>
+      <c r="AJ10" s="19"/>
+      <c r="AK10" s="19"/>
     </row>
     <row r="11" spans="1:37" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="23">
+      <c r="D11" s="21">
         <v>1</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="26">
         <v>2</v>
       </c>
       <c r="F11" s="3">
@@ -934,319 +949,275 @@
       <c r="W12" s="4"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:37" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="17"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="J18" s="17"/>
+      <c r="G18" s="5"/>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="I19" s="20"/>
-      <c r="K19" s="24"/>
+      <c r="C19" s="8"/>
+      <c r="I19" s="13"/>
+      <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
+      <c r="C20" s="8"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
+      <c r="I21" s="13"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="19"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N24" s="13"/>
+      <c r="N24" s="1"/>
       <c r="O24" s="5"/>
-      <c r="Q24" s="24"/>
+      <c r="Q24" s="15"/>
     </row>
     <row r="25" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
-      <c r="V25" s="17"/>
-      <c r="W25" s="19"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
     </row>
     <row r="26" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="17"/>
-      <c r="W26" s="19"/>
+      <c r="V26" s="12"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="W27" s="24"/>
+      <c r="W27" s="15"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="8"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="8"/>
+      <c r="W28" s="20"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="17"/>
-      <c r="V28" s="17"/>
-      <c r="W28" s="17"/>
-    </row>
-    <row r="29" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="12"/>
-    </row>
-    <row r="31" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="10" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+    </row>
+    <row r="30" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B6:F6"/>

</xml_diff>